<commit_message>
- add kerf test module - large refactoring to make most options available on command line
</commit_message>
<xml_diff>
--- a/Table-tagsizes.xlsx
+++ b/Table-tagsizes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16400" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>mm per inch</t>
   </si>
@@ -79,6 +79,18 @@
   </si>
   <si>
     <t>campix/tagpix</t>
+  </si>
+  <si>
+    <t>medium cut</t>
+  </si>
+  <si>
+    <t>tag2 mm</t>
+  </si>
+  <si>
+    <t>vlc1 videos</t>
+  </si>
+  <si>
+    <t>Gurabo 19 videos</t>
   </si>
 </sst>
 </file>
@@ -129,7 +141,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,6 +169,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF66CCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF80FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -232,7 +262,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -333,9 +363,6 @@
     <xf numFmtId="171" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="171" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -346,6 +373,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -695,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:L35"/>
+  <dimension ref="A3:M35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -706,11 +751,11 @@
     <col min="2" max="4" width="16.5" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" customWidth="1"/>
-    <col min="10" max="10" width="13.5" customWidth="1"/>
+    <col min="9" max="10" width="11.83203125" customWidth="1"/>
+    <col min="11" max="11" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -718,7 +763,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -727,7 +772,7 @@
         <v>2.1166666666666667E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:13">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="3" t="s">
@@ -747,14 +792,17 @@
         <v>16</v>
       </c>
       <c r="I6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="24"/>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="24"/>
+      <c r="L6" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:13">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -780,17 +828,20 @@
         <v>12</v>
       </c>
       <c r="I7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="K7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="40" t="s">
+      <c r="L7" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="25"/>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7" s="25"/>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="2">
         <f>B8*B8</f>
         <v>25</v>
@@ -821,20 +872,24 @@
         <f>F8*D8</f>
         <v>1.3334999999999999</v>
       </c>
-      <c r="I8" s="38">
+      <c r="I8" s="5">
+        <f>F8*(C8+4)</f>
+        <v>1.6298333333333335</v>
+      </c>
+      <c r="J8" s="37">
         <f>F8*(C8+6)</f>
         <v>1.9261666666666666</v>
       </c>
-      <c r="J8" s="16">
-        <f t="shared" ref="J8:J14" si="0">30*G8/1.6</f>
+      <c r="K8" s="16">
+        <f t="shared" ref="K8:K14" si="0">30*G8/1.6</f>
         <v>19.446874999999999</v>
       </c>
-      <c r="K8" s="28">
-        <f>J8/C8</f>
+      <c r="L8" s="28">
+        <f>K8/C8</f>
         <v>2.7781249999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:13">
       <c r="A9" s="2">
         <f>B9*B9</f>
         <v>25</v>
@@ -865,22 +920,26 @@
         <f>F9*D9</f>
         <v>1.524</v>
       </c>
-      <c r="I9" s="38">
-        <f t="shared" ref="I9:I35" si="1">F9*(C9+6)</f>
+      <c r="I9" s="7">
+        <f t="shared" ref="I9:I35" si="1">F9*(C9+4)</f>
+        <v>1.8626666666666667</v>
+      </c>
+      <c r="J9" s="37">
+        <f t="shared" ref="J9:J35" si="2">F9*(C9+6)</f>
         <v>2.2013333333333334</v>
       </c>
-      <c r="J9" s="16">
+      <c r="K9" s="16">
         <f t="shared" si="0"/>
         <v>22.225000000000001</v>
       </c>
-      <c r="K9" s="28">
-        <f t="shared" ref="K9:K35" si="2">J9/C9</f>
+      <c r="L9" s="28">
+        <f t="shared" ref="L9:L35" si="3">K9/C9</f>
         <v>3.1750000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:13">
       <c r="A10" s="2">
-        <f>B10*B10</f>
+        <f t="shared" ref="A10:A21" si="4">B10*B10</f>
         <v>25</v>
       </c>
       <c r="B10" s="18">
@@ -894,7 +953,7 @@
         <f>C10+2</f>
         <v>9</v>
       </c>
-      <c r="E10" s="31">
+      <c r="E10" s="41">
         <v>9</v>
       </c>
       <c r="F10" s="5">
@@ -909,22 +968,26 @@
         <f>F10*D10</f>
         <v>1.7145000000000001</v>
       </c>
-      <c r="I10" s="33">
-        <f t="shared" si="1"/>
+      <c r="I10" s="42">
+        <f t="shared" si="1"/>
+        <v>2.0954999999999999</v>
+      </c>
+      <c r="J10" s="42">
+        <f t="shared" si="2"/>
         <v>2.4765000000000001</v>
       </c>
-      <c r="J10" s="16">
+      <c r="K10" s="16">
         <f t="shared" si="0"/>
         <v>25.003124999999997</v>
       </c>
-      <c r="K10" s="27">
-        <f t="shared" si="2"/>
+      <c r="L10" s="40">
+        <f t="shared" si="3"/>
         <v>3.5718749999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:13">
       <c r="A11" s="2">
-        <f>B11*B11</f>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="B11" s="18">
@@ -938,7 +1001,7 @@
         <f>C11+2</f>
         <v>9</v>
       </c>
-      <c r="E11" s="31">
+      <c r="E11" s="41">
         <v>10</v>
       </c>
       <c r="F11" s="5">
@@ -949,26 +1012,30 @@
         <f>F11*C11</f>
         <v>1.4816666666666667</v>
       </c>
-      <c r="H11" s="38">
+      <c r="H11" s="37">
         <f>F11*D11</f>
         <v>1.905</v>
       </c>
-      <c r="I11" s="33">
-        <f t="shared" si="1"/>
+      <c r="I11" s="42">
+        <f t="shared" si="1"/>
+        <v>2.3283333333333331</v>
+      </c>
+      <c r="J11" s="33">
+        <f t="shared" si="2"/>
         <v>2.7516666666666669</v>
       </c>
-      <c r="J11" s="16">
+      <c r="K11" s="16">
         <f t="shared" si="0"/>
         <v>27.78125</v>
       </c>
-      <c r="K11" s="27">
-        <f t="shared" si="2"/>
+      <c r="L11" s="40">
+        <f t="shared" si="3"/>
         <v>3.96875</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:13">
       <c r="A12" s="2">
-        <f>B12*B12</f>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="B12" s="18">
@@ -993,25 +1060,30 @@
         <f>F12*C12</f>
         <v>1.6298333333333335</v>
       </c>
-      <c r="H12" s="38">
+      <c r="H12" s="37">
         <f>F12*D12</f>
         <v>2.0954999999999999</v>
       </c>
       <c r="I12" s="5">
         <f t="shared" si="1"/>
+        <v>2.5611666666666668</v>
+      </c>
+      <c r="J12" s="5">
+        <f t="shared" si="2"/>
         <v>3.0268333333333333</v>
       </c>
-      <c r="J12" s="16">
-        <f t="shared" ref="J12" si="3">30*G12/1.6</f>
+      <c r="K12" s="16">
+        <f t="shared" ref="K12" si="5">30*G12/1.6</f>
         <v>30.559374999999999</v>
       </c>
-      <c r="K12" s="28">
-        <f t="shared" ref="K12" si="4">J12/C12</f>
+      <c r="L12" s="28">
+        <f t="shared" ref="L12" si="6">K12/C12</f>
         <v>4.3656249999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:13">
       <c r="A13" s="2">
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="B13" s="19">
@@ -1042,19 +1114,24 @@
       </c>
       <c r="I13" s="5">
         <f t="shared" si="1"/>
+        <v>2.1999999999999997</v>
+      </c>
+      <c r="J13" s="5">
+        <f t="shared" si="2"/>
         <v>2.5999999999999996</v>
       </c>
-      <c r="J13" s="16">
+      <c r="K13" s="16">
         <f t="shared" si="0"/>
         <v>26.25</v>
       </c>
-      <c r="K13" s="27">
-        <f t="shared" si="2"/>
+      <c r="L13" s="27">
+        <f t="shared" si="3"/>
         <v>3.75</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:13">
       <c r="A14" s="2">
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="B14" s="19">
@@ -1085,19 +1162,24 @@
       </c>
       <c r="I14" s="5">
         <f t="shared" si="1"/>
+        <v>2.3571428571428572</v>
+      </c>
+      <c r="J14" s="5">
+        <f t="shared" si="2"/>
         <v>2.7857142857142856</v>
       </c>
-      <c r="J14" s="16">
+      <c r="K14" s="16">
         <f t="shared" si="0"/>
         <v>28.125</v>
       </c>
-      <c r="K14" s="28">
-        <f t="shared" si="2"/>
+      <c r="L14" s="28">
+        <f t="shared" si="3"/>
         <v>4.0178571428571432</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:13">
       <c r="A15" s="2">
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="B15" s="19">
@@ -1128,19 +1210,24 @@
       </c>
       <c r="I15" s="5">
         <f t="shared" si="1"/>
+        <v>2.5142857142857147</v>
+      </c>
+      <c r="J15" s="5">
+        <f t="shared" si="2"/>
         <v>2.9714285714285715</v>
       </c>
-      <c r="J15" s="16">
+      <c r="K15" s="16">
         <f>30*G15/1.6</f>
         <v>30</v>
       </c>
-      <c r="K15" s="28">
-        <f t="shared" si="2"/>
+      <c r="L15" s="28">
+        <f t="shared" si="3"/>
         <v>4.2857142857142856</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:13">
       <c r="A16" s="2">
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="B16" s="19">
@@ -1171,19 +1258,24 @@
       </c>
       <c r="I16" s="5">
         <f t="shared" si="1"/>
+        <v>2.6714285714285713</v>
+      </c>
+      <c r="J16" s="5">
+        <f t="shared" si="2"/>
         <v>3.157142857142857</v>
       </c>
-      <c r="J16" s="16">
-        <f t="shared" ref="J16:J35" si="5">30*G16/1.6</f>
+      <c r="K16" s="16">
+        <f t="shared" ref="K16:K35" si="7">30*G16/1.6</f>
         <v>31.875</v>
       </c>
-      <c r="K16" s="28">
-        <f t="shared" si="2"/>
+      <c r="L16" s="28">
+        <f t="shared" si="3"/>
         <v>4.5535714285714288</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:13">
       <c r="A17" s="2">
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="B17" s="19">
@@ -1214,19 +1306,24 @@
       </c>
       <c r="I17" s="5">
         <f t="shared" si="1"/>
+        <v>1.9555555555555557</v>
+      </c>
+      <c r="J17" s="5">
+        <f t="shared" si="2"/>
         <v>2.3111111111111113</v>
       </c>
-      <c r="J17" s="16">
-        <f t="shared" si="5"/>
+      <c r="K17" s="16">
+        <f t="shared" si="7"/>
         <v>23.333333333333332</v>
       </c>
-      <c r="K17" s="28">
-        <f t="shared" si="2"/>
+      <c r="L17" s="28">
+        <f t="shared" si="3"/>
         <v>3.333333333333333</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:13">
       <c r="A18" s="2">
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="B18" s="19">
@@ -1257,19 +1354,24 @@
       </c>
       <c r="I18" s="5">
         <f t="shared" si="1"/>
+        <v>2.0777777777777775</v>
+      </c>
+      <c r="J18" s="5">
+        <f t="shared" si="2"/>
         <v>2.4555555555555557</v>
       </c>
-      <c r="J18" s="16">
-        <f t="shared" si="5"/>
+      <c r="K18" s="16">
+        <f t="shared" si="7"/>
         <v>24.791666666666664</v>
       </c>
-      <c r="K18" s="28">
-        <f t="shared" si="2"/>
+      <c r="L18" s="28">
+        <f t="shared" si="3"/>
         <v>3.5416666666666665</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:13">
       <c r="A19" s="2">
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="B19" s="19">
@@ -1300,19 +1402,24 @@
       </c>
       <c r="I19" s="5">
         <f t="shared" si="1"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J19" s="5">
+        <f t="shared" si="2"/>
         <v>2.6</v>
       </c>
-      <c r="J19" s="16">
-        <f t="shared" si="5"/>
+      <c r="K19" s="16">
+        <f t="shared" si="7"/>
         <v>26.250000000000004</v>
       </c>
-      <c r="K19" s="27">
-        <f t="shared" si="2"/>
+      <c r="L19" s="27">
+        <f t="shared" si="3"/>
         <v>3.7500000000000004</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:13">
       <c r="A20" s="2">
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="B20" s="19">
@@ -1343,19 +1450,24 @@
       </c>
       <c r="I20" s="5">
         <f t="shared" si="1"/>
+        <v>2.3222222222222224</v>
+      </c>
+      <c r="J20" s="5">
+        <f t="shared" si="2"/>
         <v>2.7444444444444445</v>
       </c>
-      <c r="J20" s="16">
-        <f t="shared" si="5"/>
+      <c r="K20" s="16">
+        <f t="shared" si="7"/>
         <v>27.708333333333332</v>
       </c>
-      <c r="K20" s="28">
-        <f t="shared" si="2"/>
+      <c r="L20" s="28">
+        <f t="shared" si="3"/>
         <v>3.958333333333333</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="16" thickBot="1">
+    <row r="21" spans="1:13" ht="16" thickBot="1">
       <c r="A21" s="10">
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="B21" s="20">
@@ -1386,18 +1498,22 @@
       </c>
       <c r="I21" s="12">
         <f t="shared" si="1"/>
+        <v>2.4444444444444442</v>
+      </c>
+      <c r="J21" s="12">
+        <f t="shared" si="2"/>
         <v>2.8888888888888888</v>
       </c>
-      <c r="J21" s="17">
-        <f t="shared" si="5"/>
+      <c r="K21" s="17">
+        <f t="shared" si="7"/>
         <v>29.166666666666661</v>
       </c>
-      <c r="K21" s="29">
-        <f t="shared" si="2"/>
+      <c r="L21" s="29">
+        <f t="shared" si="3"/>
         <v>4.1666666666666661</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:13">
       <c r="A22" s="8">
         <f>B22*B22</f>
         <v>36</v>
@@ -1428,20 +1544,24 @@
         <f>F22*D22</f>
         <v>1.4816666666666667</v>
       </c>
-      <c r="I22" s="39">
-        <f t="shared" si="1"/>
+      <c r="I22" s="9">
+        <f t="shared" si="1"/>
+        <v>1.778</v>
+      </c>
+      <c r="J22" s="38">
+        <f t="shared" si="2"/>
         <v>2.0743333333333336</v>
       </c>
-      <c r="J22" s="26">
-        <f t="shared" si="5"/>
+      <c r="K22" s="26">
+        <f t="shared" si="7"/>
         <v>22.225000000000001</v>
       </c>
-      <c r="K22" s="30">
-        <f t="shared" si="2"/>
+      <c r="L22" s="30">
+        <f t="shared" si="3"/>
         <v>2.7781250000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:13">
       <c r="A23" s="2">
         <f>B23*B23</f>
         <v>36</v>
@@ -1472,20 +1592,24 @@
         <f>F23*D23</f>
         <v>1.6933333333333334</v>
       </c>
-      <c r="I23" s="5">
-        <f t="shared" si="1"/>
+      <c r="I23" s="37">
+        <f t="shared" si="1"/>
+        <v>2.032</v>
+      </c>
+      <c r="J23" s="5">
+        <f t="shared" si="2"/>
         <v>2.3706666666666667</v>
       </c>
-      <c r="J23" s="16">
-        <f t="shared" si="5"/>
+      <c r="K23" s="16">
+        <f t="shared" si="7"/>
         <v>25.4</v>
       </c>
-      <c r="K23" s="28">
-        <f t="shared" si="2"/>
+      <c r="L23" s="28">
+        <f t="shared" si="3"/>
         <v>3.1749999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:13">
       <c r="A24" s="2">
         <f>B24*B24</f>
         <v>36</v>
@@ -1501,7 +1625,7 @@
         <f>C24+2</f>
         <v>10</v>
       </c>
-      <c r="E24" s="31">
+      <c r="E24" s="41">
         <v>9</v>
       </c>
       <c r="F24" s="5">
@@ -1512,24 +1636,28 @@
         <f>F24*C24</f>
         <v>1.524</v>
       </c>
-      <c r="H24" s="38">
+      <c r="H24" s="37">
         <f>F24*D24</f>
         <v>1.905</v>
       </c>
-      <c r="I24" s="33">
-        <f t="shared" si="1"/>
+      <c r="I24" s="5">
+        <f t="shared" si="1"/>
+        <v>2.286</v>
+      </c>
+      <c r="J24" s="33">
+        <f t="shared" si="2"/>
         <v>2.6669999999999998</v>
       </c>
-      <c r="J24" s="16">
-        <f t="shared" si="5"/>
+      <c r="K24" s="16">
+        <f t="shared" si="7"/>
         <v>28.574999999999999</v>
       </c>
-      <c r="K24" s="27">
-        <f t="shared" si="2"/>
+      <c r="L24" s="40">
+        <f t="shared" si="3"/>
         <v>3.5718749999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:13">
       <c r="A25" s="2">
         <f>B25*B25</f>
         <v>36</v>
@@ -1545,7 +1673,7 @@
         <f>C25+2</f>
         <v>10</v>
       </c>
-      <c r="E25" s="31">
+      <c r="E25" s="41">
         <v>10</v>
       </c>
       <c r="F25" s="5">
@@ -1556,26 +1684,30 @@
         <f>F25*C25</f>
         <v>1.6933333333333334</v>
       </c>
-      <c r="H25" s="38">
+      <c r="H25" s="37">
         <f>F25*D25</f>
         <v>2.1166666666666667</v>
       </c>
-      <c r="I25" s="33">
-        <f t="shared" si="1"/>
+      <c r="I25" s="5">
+        <f t="shared" si="1"/>
+        <v>2.54</v>
+      </c>
+      <c r="J25" s="33">
+        <f t="shared" si="2"/>
         <v>2.9633333333333334</v>
       </c>
-      <c r="J25" s="16">
-        <f t="shared" si="5"/>
+      <c r="K25" s="16">
+        <f t="shared" si="7"/>
         <v>31.749999999999996</v>
       </c>
-      <c r="K25" s="27">
-        <f t="shared" si="2"/>
+      <c r="L25" s="40">
+        <f t="shared" si="3"/>
         <v>3.9687499999999996</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:13">
       <c r="A26" s="2">
-        <f>B26*B26</f>
+        <f t="shared" ref="A26:A35" si="8">B26*B26</f>
         <v>36</v>
       </c>
       <c r="B26" s="18">
@@ -1606,20 +1738,25 @@
       </c>
       <c r="I26" s="5">
         <f t="shared" si="1"/>
+        <v>2.794</v>
+      </c>
+      <c r="J26" s="5">
+        <f t="shared" si="2"/>
         <v>3.2596666666666669</v>
       </c>
-      <c r="J26" s="16">
-        <f t="shared" si="5"/>
+      <c r="K26" s="16">
+        <f t="shared" si="7"/>
         <v>34.924999999999997</v>
       </c>
-      <c r="K26" s="28">
-        <f t="shared" si="2"/>
+      <c r="L26" s="28">
+        <f t="shared" si="3"/>
         <v>4.3656249999999996</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:13">
       <c r="A27" s="2">
-        <v>25</v>
+        <f t="shared" si="8"/>
+        <v>36</v>
       </c>
       <c r="B27" s="18">
         <v>6</v>
@@ -1640,29 +1777,37 @@
         <f>G27/C27</f>
         <v>0.17499999999999999</v>
       </c>
-      <c r="G27" s="36">
+      <c r="G27" s="45">
         <v>1.4</v>
       </c>
       <c r="H27" s="7">
         <f>F27*D27</f>
         <v>1.75</v>
       </c>
-      <c r="I27" s="5">
-        <f t="shared" si="1"/>
+      <c r="I27" s="7">
+        <f t="shared" si="1"/>
+        <v>2.0999999999999996</v>
+      </c>
+      <c r="J27" s="43">
+        <f t="shared" si="2"/>
         <v>2.4499999999999997</v>
       </c>
-      <c r="J27" s="16">
-        <f t="shared" si="5"/>
+      <c r="K27" s="16">
+        <f t="shared" si="7"/>
         <v>26.25</v>
       </c>
-      <c r="K27" s="37">
-        <f t="shared" si="2"/>
+      <c r="L27" s="36">
+        <f t="shared" si="3"/>
         <v>3.28125</v>
       </c>
-    </row>
-    <row r="28" spans="1:11">
+      <c r="M27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" s="2">
-        <v>25</v>
+        <f t="shared" si="8"/>
+        <v>36</v>
       </c>
       <c r="B28" s="18">
         <v>6</v>
@@ -1690,22 +1835,27 @@
         <f>F28*D28</f>
         <v>1.875</v>
       </c>
-      <c r="I28" s="5">
-        <f t="shared" si="1"/>
+      <c r="I28" s="7">
+        <f t="shared" si="1"/>
+        <v>2.25</v>
+      </c>
+      <c r="J28" s="5">
+        <f t="shared" si="2"/>
         <v>2.625</v>
       </c>
-      <c r="J28" s="16">
-        <f t="shared" si="5"/>
+      <c r="K28" s="16">
+        <f t="shared" si="7"/>
         <v>28.125</v>
       </c>
-      <c r="K28" s="28">
-        <f t="shared" si="2"/>
+      <c r="L28" s="28">
+        <f t="shared" si="3"/>
         <v>3.515625</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:13">
       <c r="A29" s="2">
-        <v>25</v>
+        <f t="shared" si="8"/>
+        <v>36</v>
       </c>
       <c r="B29" s="18">
         <v>6</v>
@@ -1729,26 +1879,34 @@
       <c r="G29" s="34">
         <v>1.6</v>
       </c>
-      <c r="H29" s="33">
+      <c r="H29" s="7">
         <f>F29*D29</f>
         <v>2</v>
       </c>
-      <c r="I29" s="5">
-        <f t="shared" si="1"/>
+      <c r="I29" s="7">
+        <f t="shared" si="1"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="J29" s="44">
+        <f t="shared" si="2"/>
         <v>2.8000000000000003</v>
       </c>
-      <c r="J29" s="16">
-        <f t="shared" si="5"/>
+      <c r="K29" s="16">
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
-      <c r="K29" s="35">
-        <f t="shared" si="2"/>
+      <c r="L29" s="35">
+        <f t="shared" si="3"/>
         <v>3.75</v>
       </c>
-    </row>
-    <row r="30" spans="1:11">
+      <c r="M29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" s="2">
-        <v>25</v>
+        <f t="shared" si="8"/>
+        <v>36</v>
       </c>
       <c r="B30" s="18">
         <v>6</v>
@@ -1778,20 +1936,25 @@
       </c>
       <c r="I30" s="5">
         <f t="shared" si="1"/>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="J30" s="5">
+        <f t="shared" si="2"/>
         <v>2.9750000000000001</v>
       </c>
-      <c r="J30" s="16">
-        <f t="shared" si="5"/>
+      <c r="K30" s="16">
+        <f t="shared" si="7"/>
         <v>31.875</v>
       </c>
-      <c r="K30" s="28">
-        <f t="shared" si="2"/>
+      <c r="L30" s="28">
+        <f t="shared" si="3"/>
         <v>3.984375</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:13">
       <c r="A31" s="2">
-        <v>25</v>
+        <f t="shared" si="8"/>
+        <v>36</v>
       </c>
       <c r="B31" s="18">
         <v>6</v>
@@ -1821,20 +1984,25 @@
       </c>
       <c r="I31" s="5">
         <f t="shared" si="1"/>
+        <v>1.92</v>
+      </c>
+      <c r="J31" s="5">
+        <f t="shared" si="2"/>
         <v>2.2400000000000002</v>
       </c>
-      <c r="J31" s="16">
-        <f t="shared" si="5"/>
+      <c r="K31" s="16">
+        <f t="shared" si="7"/>
         <v>23.999999999999996</v>
       </c>
-      <c r="K31" s="28">
-        <f t="shared" si="2"/>
+      <c r="L31" s="28">
+        <f t="shared" si="3"/>
         <v>2.9999999999999996</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:13">
       <c r="A32" s="2">
-        <v>25</v>
+        <f t="shared" si="8"/>
+        <v>36</v>
       </c>
       <c r="B32" s="18">
         <v>6</v>
@@ -1864,20 +2032,25 @@
       </c>
       <c r="I32" s="5">
         <f t="shared" si="1"/>
+        <v>2.04</v>
+      </c>
+      <c r="J32" s="5">
+        <f t="shared" si="2"/>
         <v>2.38</v>
       </c>
-      <c r="J32" s="16">
-        <f t="shared" si="5"/>
+      <c r="K32" s="16">
+        <f t="shared" si="7"/>
         <v>25.499999999999996</v>
       </c>
-      <c r="K32" s="28">
-        <f t="shared" si="2"/>
+      <c r="L32" s="28">
+        <f t="shared" si="3"/>
         <v>3.1874999999999996</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:12">
       <c r="A33" s="2">
-        <v>25</v>
+        <f t="shared" si="8"/>
+        <v>36</v>
       </c>
       <c r="B33" s="18">
         <v>6</v>
@@ -1907,20 +2080,25 @@
       </c>
       <c r="I33" s="5">
         <f t="shared" si="1"/>
+        <v>2.16</v>
+      </c>
+      <c r="J33" s="5">
+        <f t="shared" si="2"/>
         <v>2.52</v>
       </c>
-      <c r="J33" s="16">
-        <f t="shared" si="5"/>
+      <c r="K33" s="16">
+        <f t="shared" si="7"/>
         <v>26.999999999999996</v>
       </c>
-      <c r="K33" s="28">
-        <f t="shared" si="2"/>
+      <c r="L33" s="28">
+        <f t="shared" si="3"/>
         <v>3.3749999999999996</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:12">
       <c r="A34" s="2">
-        <v>25</v>
+        <f t="shared" si="8"/>
+        <v>36</v>
       </c>
       <c r="B34" s="18">
         <v>6</v>
@@ -1950,20 +2128,25 @@
       </c>
       <c r="I34" s="5">
         <f t="shared" si="1"/>
+        <v>2.2800000000000002</v>
+      </c>
+      <c r="J34" s="5">
+        <f t="shared" si="2"/>
         <v>2.66</v>
       </c>
-      <c r="J34" s="16">
-        <f t="shared" si="5"/>
+      <c r="K34" s="16">
+        <f t="shared" si="7"/>
         <v>28.5</v>
       </c>
-      <c r="K34" s="28">
-        <f t="shared" si="2"/>
+      <c r="L34" s="28">
+        <f t="shared" si="3"/>
         <v>3.5625</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:12">
       <c r="A35" s="2">
-        <v>25</v>
+        <f t="shared" si="8"/>
+        <v>36</v>
       </c>
       <c r="B35" s="18">
         <v>6</v>
@@ -1993,14 +2176,18 @@
       </c>
       <c r="I35" s="5">
         <f t="shared" si="1"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="J35" s="5">
+        <f t="shared" si="2"/>
         <v>2.8000000000000003</v>
       </c>
-      <c r="J35" s="28">
-        <f t="shared" si="5"/>
+      <c r="K35" s="28">
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
-      <c r="K35" s="28">
-        <f t="shared" si="2"/>
+      <c r="L35" s="28">
+        <f t="shared" si="3"/>
         <v>3.75</v>
       </c>
     </row>

</xml_diff>